<commit_message>
Connexion deconnexion OK roles
</commit_message>
<xml_diff>
--- a/hsp_java/project/GanttV1.xlsx
+++ b/hsp_java/project/GanttV1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D83240-B39A-4CA7-A319-48C545185C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09B99EE-9B83-469A-B695-B88EF102CF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2051,7 +2051,7 @@
   <dimension ref="A1:BK46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3012,7 +3012,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="53">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E9" s="24">
         <v>44572</v>
@@ -3255,7 +3255,7 @@
         <v>43</v>
       </c>
       <c r="D10" s="53">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E10" s="24">
         <v>44572</v>
@@ -3498,7 +3498,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="53">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E11" s="24">
         <v>44572</v>
@@ -3741,7 +3741,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="53">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E12" s="24">
         <v>44579</v>
@@ -3984,7 +3984,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="24">
         <v>44579</v>
@@ -5183,235 +5183,237 @@
         <v>43</v>
       </c>
       <c r="D18" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="24">
-        <v>44586</v>
-      </c>
-      <c r="F18" s="45"/>
+        <v>44579</v>
+      </c>
+      <c r="F18" s="45">
+        <v>1</v>
+      </c>
       <c r="G18" s="20"/>
       <c r="H18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="I18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="J18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="K18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="L18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="M18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="N18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="O18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P18" s="27">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <v>1</v>
       </c>
       <c r="Q18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="R18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="S18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="T18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="U18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="V18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="W18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="X18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Y18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Z18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AA18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AB18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AC18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AD18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AE18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AF18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AG18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AH18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AI18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AJ18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AK18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AL18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AM18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AN18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AO18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AP18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AQ18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AR18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AS18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AT18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AU18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AV18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AW18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AX18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AY18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AZ18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BA18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BB18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BC18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BD18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BE18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BF18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BG18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BH18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BI18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BJ18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BK18" s="27" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E18,$F18=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>